<commit_message>
Added SonarLint analysis and updates.
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrei\Documents\GitHub\aair2650VVSS\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Facultate\New\AnulIV\SemII\VVSS\Lab\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13618E3-0D98-4CF9-AD86-3410C7DFC73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDD225A-65EB-4D3D-A10E-FEDD34483E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="84">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -217,34 +215,76 @@
     <t>Multe dintre asocieri si agregari nu au denumiri.</t>
   </si>
   <si>
-    <t>C09</t>
-  </si>
-  <si>
-    <t>Part line 16</t>
-  </si>
-  <si>
-    <t>Nu este clar ce semnifica parametrii min si max din constructor</t>
-  </si>
-  <si>
-    <t>C07</t>
-  </si>
-  <si>
-    <t>ModifyProductController line 259</t>
-  </si>
-  <si>
-    <t>Nu se intampla nimic in cazul in care se da search la un produs inexistent</t>
-  </si>
-  <si>
-    <t>C04</t>
-  </si>
-  <si>
-    <t>AddPartController line 172</t>
-  </si>
-  <si>
-    <t>In cazul in care se introduce o valoare numerica invalida se afiseaza eronat mesajul "Form contains blank field"</t>
-  </si>
-  <si>
-    <t>AddProductController line 220</t>
+    <t>SonarLint</t>
+  </si>
+  <si>
+    <t>5.03.2022</t>
+  </si>
+  <si>
+    <t>AddPartController,28</t>
+  </si>
+  <si>
+    <t>Private field partId not used</t>
+  </si>
+  <si>
+    <t>private int partId;</t>
+  </si>
+  <si>
+    <t>AddProductController,151</t>
+  </si>
+  <si>
+    <t>isPresent() should be called</t>
+  </si>
+  <si>
+    <t>if (result.get() == ButtonType.OK)</t>
+  </si>
+  <si>
+    <t>Removed line</t>
+  </si>
+  <si>
+    <t>if(result.isPresent())</t>
+  </si>
+  <si>
+    <t>AddProductController,31</t>
+  </si>
+  <si>
+    <t>Private field productId not used</t>
+  </si>
+  <si>
+    <t>private int productId;</t>
+  </si>
+  <si>
+    <t>AddProductController,174</t>
+  </si>
+  <si>
+    <t>AddPartController,108</t>
+  </si>
+  <si>
+    <t>Part,16</t>
+  </si>
+  <si>
+    <t>Constructor should be protected since Part is an abstract class</t>
+  </si>
+  <si>
+    <t>public Part(int partId, String name, double price, int inStock, int min, int max) {</t>
+  </si>
+  <si>
+    <t>protected Part(int partId, String name, double price, int inStock, int min, int max) {</t>
+  </si>
+  <si>
+    <t>AddPartController,165</t>
+  </si>
+  <si>
+    <t>Remove unnecesarry boolean literal</t>
+  </si>
+  <si>
+    <t>if(isOutsourced == true)</t>
+  </si>
+  <si>
+    <t>Even if it is not necesarry, it makes the code easier to read so we will keep it</t>
+  </si>
+  <si>
+    <t>ModifyPartController,34</t>
   </si>
 </sst>
 </file>
@@ -436,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -513,6 +553,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,7 +900,7 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -1198,8 +1242,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,9 +1541,7 @@
         <v>8</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="E28" s="1">
-        <v>0.5</v>
-      </c>
+      <c r="E28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1522,8 +1564,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,7 +1573,7 @@
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
@@ -1640,64 +1682,40 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>68</v>
-      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
@@ -1860,9 +1878,7 @@
         <v>8</v>
       </c>
       <c r="D32" s="13"/>
-      <c r="E32" s="1">
-        <v>0.5</v>
-      </c>
+      <c r="E32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1885,18 +1901,18 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
+    <col min="3" max="3" width="23" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" style="6" customWidth="1"/>
     <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="6"/>
@@ -1943,7 +1959,9 @@
       <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="33"/>
+      <c r="D4" s="33" t="s">
+        <v>60</v>
+      </c>
       <c r="E4" s="33"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
@@ -1959,7 +1977,9 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="23" t="s">
+        <v>49</v>
+      </c>
       <c r="E5" s="23"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
@@ -1976,7 +1996,9 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="23" t="s">
+        <v>61</v>
+      </c>
       <c r="E6" s="23"/>
       <c r="F6" s="21"/>
     </row>
@@ -1997,84 +2019,148 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="C17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
@@ -2215,7 +2301,9 @@
       </c>
       <c r="D32" s="37"/>
       <c r="E32" s="37"/>
-      <c r="F32" s="19"/>
+      <c r="F32" s="19">
+        <v>0.25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>